<commit_message>
tblSponsoren Aktivitaets-Toggels fuer die Sponsoren gesetzt.
</commit_message>
<xml_diff>
--- a/0-Datengrundlage/3-Pate/!-Pate-Gesamt.xlsx
+++ b/0-Datengrundlage/3-Pate/!-Pate-Gesamt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tricuper\Documents\GitHub\TTSF-Hohberg-Sponsoring\0-Datengrundlage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tricuper\Documents\GitHub\TTSF-Hohberg-Sponsoring\0-Datengrundlage\3-Pate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506D52C7-919E-404B-A57E-331A0D31A70F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E453DFD-3D79-4991-88F3-1AB7EB77E275}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7215" yWindow="2820" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle3" sheetId="3" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>Adelbert Bußhardt</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>Paten_Name</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,107 +421,107 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>